<commit_message>
added late to eff group
</commit_message>
<xml_diff>
--- a/output/processed_data.xlsx
+++ b/output/processed_data.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,36 +470,140 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C2" t="n">
-        <v>11.52</v>
+        <v>13.98963730569948</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C3" t="n">
-        <v>17.76</v>
+        <v>8.393782383419689</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B4" t="n">
+        <v>161</v>
+      </c>
+      <c r="C4" t="n">
+        <v>50.05181347150259</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DIAN4065.ENTRIALGO</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>27</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8.393782383419689</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>LOANA.MBONGO</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>48</v>
+      </c>
+      <c r="C6" t="n">
+        <v>14.92227979274611</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MICA0432.RIZKALLAMAR</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>52</v>
+      </c>
+      <c r="C7" t="n">
+        <v>16.16580310880829</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PATR5027.AMEH</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.96</v>
+      <c r="C8" t="n">
+        <v>0.6217616580310881</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SURESH.DHAWAN</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>99</v>
+      </c>
+      <c r="C9" t="n">
+        <v>30.77720207253886</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>THIE6554.DIALLO</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>106</v>
+      </c>
+      <c r="C10" t="n">
+        <v>32.95336787564766</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>TUSHAR.BHATIA</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>23</v>
+      </c>
+      <c r="C11" t="n">
+        <v>7.150259067357513</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ZAHIDGUL.MINHAS</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.55440414507772</v>
       </c>
     </row>
   </sheetData>
@@ -513,7 +617,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,53 +645,92 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ASHA1141.PAGE</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>7.68</v>
+        <v>0.310880829015544</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>7.199999999999999</v>
+        <v>2.797927461139896</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C4" t="n">
-        <v>0.48</v>
+        <v>16.78756476683938</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>0.48</v>
+        <v>2.487046632124352</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PATR5027.AMEH</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.243523316062176</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>30</v>
+      </c>
+      <c r="C7" t="n">
+        <v>9.326424870466321</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ZAHIDGUL.MINHAS</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.243523316062176</v>
       </c>
     </row>
   </sheetData>
@@ -601,7 +744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,79 +772,92 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C2" t="n">
-        <v>2.4</v>
+        <v>10.88082901554404</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>128</v>
+        <v>14</v>
       </c>
       <c r="C3" t="n">
-        <v>61.44</v>
+        <v>4.352331606217616</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C4" t="n">
-        <v>2.4</v>
+        <v>15.5440414507772</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>SEPIDEH.AZARIHASHJIN</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>153</v>
       </c>
       <c r="C5" t="n">
-        <v>3.36</v>
+        <v>47.56476683937824</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="C6" t="n">
-        <v>24.48</v>
+        <v>26.73575129533679</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>TUSHAR.BHATIA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>6.239999999999999</v>
+        <v>3.730569948186528</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>15</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4.66321243523316</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +871,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -743,27 +899,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33</v>
+        <v>170</v>
       </c>
       <c r="C2" t="n">
-        <v>15.84</v>
+        <v>52.84974093264248</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ANJALI.BAKSHI</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="C3" t="n">
-        <v>1.44</v>
+        <v>25.49222797927461</v>
       </c>
     </row>
     <row r="4">
@@ -773,10 +929,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C4" t="n">
-        <v>2.88</v>
+        <v>7.150259067357513</v>
       </c>
     </row>
     <row r="5">
@@ -786,192 +942,257 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>29</v>
+        <v>112</v>
       </c>
       <c r="C5" t="n">
-        <v>13.92</v>
+        <v>34.81865284974093</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="C6" t="n">
-        <v>25.92</v>
+        <v>27.04663212435233</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C7" t="n">
-        <v>39.84</v>
+        <v>28.29015544041451</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="C8" t="n">
-        <v>23.04</v>
+        <v>22.69430051813471</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>INUK4091.QAVAVAU</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C9" t="n">
-        <v>51.36</v>
+        <v>29.84455958549223</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C10" t="n">
-        <v>46.08</v>
+        <v>26.1139896373057</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C11" t="n">
-        <v>17.28</v>
+        <v>15.5440414507772</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C12" t="n">
-        <v>20.64</v>
+        <v>17.72020725388601</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C13" t="n">
-        <v>1.44</v>
+        <v>11.50259067357513</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="C14" t="n">
-        <v>35.04</v>
+        <v>32.02072538860104</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C15" t="n">
-        <v>26.4</v>
+        <v>23.62694300518135</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C16" t="n">
-        <v>2.4</v>
+        <v>18.96373056994819</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="C17" t="n">
-        <v>30.24</v>
+        <v>31.39896373056995</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="C18" t="n">
-        <v>45.59999999999999</v>
+        <v>10.25906735751295</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="C19" t="n">
-        <v>1.44</v>
+        <v>26.42487046632124</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TUSHAR.BHATIA</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>99</v>
+      </c>
+      <c r="C20" t="n">
+        <v>30.77720207253886</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>83</v>
+      </c>
+      <c r="C21" t="n">
+        <v>25.80310880829015</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>WILDINE.JEUNE</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>172</v>
+      </c>
+      <c r="C22" t="n">
+        <v>53.47150259067357</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>112</v>
+      </c>
+      <c r="C23" t="n">
+        <v>34.81865284974093</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ZAKI0190.PHILLIPHORS</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>118</v>
+      </c>
+      <c r="C24" t="n">
+        <v>36.68393782383419</v>
       </c>
     </row>
   </sheetData>
@@ -985,7 +1206,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1017,114 +1238,166 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>113</v>
+        <v>173</v>
       </c>
       <c r="C2" t="n">
-        <v>54.23999999999999</v>
+        <v>53.78238341968912</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C3" t="n">
-        <v>36.48</v>
+        <v>24.55958549222798</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ESSE0616.UDEH</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="C4" t="n">
-        <v>41.27999999999999</v>
+        <v>10.25906735751295</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MARI882N.ABDELKADER</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="C5" t="n">
-        <v>59.52</v>
+        <v>47.87564766839378</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>ESSE0616.UDEH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>321</v>
       </c>
       <c r="C6" t="n">
-        <v>3.84</v>
+        <v>99.79274611398964</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>7.68</v>
+        <v>3.10880829015544</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>25</v>
+        <v>171</v>
       </c>
       <c r="C8" t="n">
-        <v>12</v>
+        <v>53.16062176165803</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="C9" t="n">
-        <v>9.6</v>
+        <v>30.15544041450777</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>STAN9294.BAUER</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>112</v>
+      </c>
+      <c r="C10" t="n">
+        <v>34.81865284974093</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SURESH.DHAWAN</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>199</v>
+      </c>
+      <c r="C11" t="n">
+        <v>61.86528497409326</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>THIE6554.DIALLO</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>86</v>
+      </c>
+      <c r="C12" t="n">
+        <v>26.73575129533679</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>WESL5337.CADETTE</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>63</v>
-      </c>
-      <c r="C10" t="n">
-        <v>30.24</v>
+      <c r="B13" t="n">
+        <v>107</v>
+      </c>
+      <c r="C13" t="n">
+        <v>33.26424870466321</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>42</v>
+      </c>
+      <c r="C14" t="n">
+        <v>13.05699481865285</v>
       </c>
     </row>
   </sheetData>
@@ -1138,7 +1411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1165,27 +1438,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>52</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ANJALI.BAKSHI</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>124</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ASHA1141.PAGE</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -1195,7 +1468,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>119</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -1205,87 +1478,87 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ESSE0616.UDEH</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>97</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>ESSE0616.UDEH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>28</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>INUK4091.QAVAVAU</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>88</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
@@ -1295,7 +1568,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>85</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16">
@@ -1305,117 +1578,147 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>124</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>49</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>117</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>SEPIDEH.AZARIHASHJIN</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>116</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>SURESH.DHAWAN</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>120</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>TUSHAR.BHATIA</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>121</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>WILDINE.JEUNE</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ZAHIDGUL.MINHAS</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>112</v>
+      <c r="B30" t="n">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1469,16 +1772,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-16</v>
+        <v>-27</v>
       </c>
       <c r="C2" t="n">
-        <v>-40</v>
+        <v>-24</v>
       </c>
       <c r="D2" t="n">
-        <v>-396</v>
+        <v>-468</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3">
@@ -1486,16 +1789,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-1</v>
+        <v>-41</v>
       </c>
       <c r="C3" t="n">
-        <v>-137</v>
+        <v>-130</v>
       </c>
       <c r="D3" t="n">
-        <v>-399</v>
+        <v>-788</v>
       </c>
       <c r="E3" t="n">
-        <v>-63</v>
+        <v>-81</v>
       </c>
     </row>
     <row r="4">
@@ -1503,16 +1806,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-16</v>
+        <v>-32</v>
       </c>
       <c r="C4" t="n">
-        <v>-32</v>
+        <v>-168</v>
       </c>
       <c r="D4" t="n">
-        <v>-40</v>
+        <v>-645</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>-357</v>
       </c>
     </row>
     <row r="5">
@@ -1520,16 +1823,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>-43</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>-104</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>-156</v>
       </c>
     </row>
     <row r="6">
@@ -1539,16 +1842,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-33</v>
+        <v>-110</v>
       </c>
       <c r="C6" t="n">
-        <v>-209</v>
+        <v>-365</v>
       </c>
       <c r="D6" t="n">
-        <v>-835</v>
+        <v>-2005</v>
       </c>
       <c r="E6" t="n">
-        <v>-63</v>
+        <v>-595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added scroll through idle times
</commit_message>
<xml_diff>
--- a/output/processed_data.xlsx
+++ b/output/processed_data.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,179 +470,140 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C2" t="n">
-        <v>26.12068965517241</v>
+        <v>13.98963730569948</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5172413793103449</v>
+        <v>8.393782383419689</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AHME0710.JUBRAN</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="C4" t="n">
-        <v>6.46551724137931</v>
+        <v>50.05181347150259</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DAT0626.LIEN</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>1.551724137931034</v>
+        <v>8.393782383419689</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>155</v>
+        <v>48</v>
       </c>
       <c r="C6" t="n">
-        <v>40.08620689655172</v>
+        <v>14.92227979274611</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>150</v>
+        <v>52</v>
       </c>
       <c r="C7" t="n">
-        <v>38.79310344827586</v>
+        <v>16.16580310880829</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>EDIT0625.DELACRUZ</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>2.586206896551724</v>
+        <v>0.6217616580310881</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>EDIT0934.TUPINO</t>
+          <t>SURESH.DHAWAN</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="C9" t="n">
-        <v>2.068965517241379</v>
+        <v>30.77720207253886</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="C10" t="n">
-        <v>1.293103448275862</v>
+        <v>32.95336787564766</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>TUSHAR.BHATIA</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5172413793103449</v>
+        <v>7.150259067357513</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>25.08620689655172</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>50</v>
-      </c>
-      <c r="C13" t="n">
-        <v>12.93103448275862</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>95</v>
-      </c>
-      <c r="C14" t="n">
-        <v>24.56896551724138</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>ZAHIDGUL.MINHAS</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>6</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1.551724137931034</v>
+        <v>1.55440414507772</v>
       </c>
     </row>
   </sheetData>
@@ -656,7 +617,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -684,14 +645,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>4.913793103448276</v>
+        <v>0.310880829015544</v>
       </c>
     </row>
     <row r="3">
@@ -701,101 +662,75 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7758620689655172</v>
+        <v>2.797927461139896</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EDGAR.JIMENEZ</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5172413793103449</v>
+        <v>16.78756476683938</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GIGNESH.PATEL</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2586206896551724</v>
+        <v>2.487046632124352</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>5.431034482758621</v>
+        <v>1.243523316062176</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C7" t="n">
-        <v>1.810344827586207</v>
+        <v>9.326424870466321</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
-        <v>22.75862068965517</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>12</v>
-      </c>
-      <c r="C9" t="n">
-        <v>3.103448275862069</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ZAHIDGUL.MINHAS</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.5172413793103449</v>
+        <v>1.243523316062176</v>
       </c>
     </row>
   </sheetData>
@@ -809,7 +744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -837,209 +772,92 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AHMAD.ALMOHAMMED</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C2" t="n">
-        <v>2.586206896551724</v>
+        <v>10.88082901554404</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C3" t="n">
-        <v>4.655172413793103</v>
+        <v>4.352331606217616</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="n">
-        <v>13.18965517241379</v>
+        <v>15.5440414507772</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FAEZ.MORADZADEH</t>
+          <t>SEPIDEH.AZARIHASHJIN</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>38</v>
+        <v>153</v>
       </c>
       <c r="C5" t="n">
-        <v>9.827586206896552</v>
+        <v>47.56476683937824</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GIGNESH.PATEL</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="C6" t="n">
-        <v>30.51724137931035</v>
+        <v>26.73575129533679</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HARDEEP.CHAUHAN</t>
+          <t>TUSHAR.BHATIA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>6.724137931034483</v>
+        <v>3.730569948186528</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C8" t="n">
-        <v>9.827586206896552</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>LOANA.MBONGO</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>4</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1.03448275862069</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>MICA0432.RIZKALLAMAR</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>34</v>
-      </c>
-      <c r="C10" t="n">
-        <v>8.793103448275861</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>NESR2403.ATTALAH</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>45</v>
-      </c>
-      <c r="C11" t="n">
-        <v>11.63793103448276</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>SRISHTI.SRISHTI</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>46</v>
-      </c>
-      <c r="C12" t="n">
-        <v>11.89655172413793</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>VICENTE.LIM</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>14</v>
-      </c>
-      <c r="C13" t="n">
-        <v>3.620689655172414</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>WESL5337.CADETTE</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>73</v>
-      </c>
-      <c r="C14" t="n">
-        <v>18.87931034482759</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>52</v>
-      </c>
-      <c r="C15" t="n">
-        <v>13.44827586206897</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>4</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1.03448275862069</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>ZEINAB.MALEKMOHAMMADI</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>27</v>
-      </c>
-      <c r="C17" t="n">
-        <v>6.982758620689655</v>
+        <v>4.66321243523316</v>
       </c>
     </row>
   </sheetData>
@@ -1053,7 +871,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1081,53 +899,53 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>25</v>
+        <v>170</v>
       </c>
       <c r="C2" t="n">
-        <v>6.46551724137931</v>
+        <v>52.84974093264248</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="C3" t="n">
-        <v>3.362068965517242</v>
+        <v>25.49222797927461</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="C4" t="n">
-        <v>17.8448275862069</v>
+        <v>7.150259067357513</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DAT0626.LIEN</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="C5" t="n">
-        <v>1.03448275862069</v>
+        <v>34.81865284974093</v>
       </c>
     </row>
     <row r="6">
@@ -1137,10 +955,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="C6" t="n">
-        <v>2.068965517241379</v>
+        <v>27.04663212435233</v>
       </c>
     </row>
     <row r="7">
@@ -1150,257 +968,231 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="C7" t="n">
-        <v>9.051724137931034</v>
+        <v>28.29015544041451</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>EDIT0625.DELACRUZ</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5172413793103449</v>
+        <v>22.69430051813471</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>EDIT0934.TUPINO</t>
+          <t>INUK4091.QAVAVAU</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="C9" t="n">
-        <v>3.103448275862069</v>
+        <v>29.84455958549223</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GIGNESH.PATEL</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="C10" t="n">
-        <v>3.103448275862069</v>
+        <v>26.1139896373057</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>172</v>
+        <v>50</v>
       </c>
       <c r="C11" t="n">
-        <v>44.48275862068966</v>
+        <v>15.5440414507772</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="C12" t="n">
-        <v>27.41379310344827</v>
+        <v>17.72020725388601</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C13" t="n">
-        <v>15.77586206896552</v>
+        <v>11.50259067357513</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C14" t="n">
-        <v>32.06896551724138</v>
+        <v>32.02072538860104</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="C15" t="n">
-        <v>29.48275862068965</v>
+        <v>23.62694300518135</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MEHD4790.FOURATI</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>258</v>
+        <v>61</v>
       </c>
       <c r="C16" t="n">
-        <v>66.72413793103448</v>
+        <v>18.96373056994819</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C17" t="n">
-        <v>23.01724137931035</v>
+        <v>31.39896373056995</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C18" t="n">
-        <v>3.103448275862069</v>
+        <v>10.25906735751295</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C19" t="n">
-        <v>10.86206896551724</v>
+        <v>26.42487046632124</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>TUSHAR.BHATIA</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="C20" t="n">
-        <v>13.70689655172414</v>
+        <v>30.77720207253886</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TARANPREET.KAUR</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C21" t="n">
-        <v>20.43103448275862</v>
+        <v>25.80310880829015</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="C22" t="n">
-        <v>16.55172413793104</v>
+        <v>53.47150259067357</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>YATI0689.YATIN</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="C23" t="n">
-        <v>21.46551724137931</v>
+        <v>34.81865284974093</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="C24" t="n">
-        <v>24.31034482758621</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>25</v>
-      </c>
-      <c r="C25" t="n">
-        <v>6.46551724137931</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>74</v>
-      </c>
-      <c r="C26" t="n">
-        <v>19.13793103448276</v>
+        <v>36.68393782383419</v>
       </c>
     </row>
   </sheetData>
@@ -1414,7 +1206,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1446,10 +1238,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="C2" t="n">
-        <v>31.03448275862069</v>
+        <v>53.78238341968912</v>
       </c>
     </row>
     <row r="3">
@@ -1459,10 +1251,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="C3" t="n">
-        <v>16.55172413793104</v>
+        <v>24.55958549222798</v>
       </c>
     </row>
     <row r="4">
@@ -1472,10 +1264,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="C4" t="n">
-        <v>25.86206896551724</v>
+        <v>10.25906735751295</v>
       </c>
     </row>
     <row r="5">
@@ -1485,10 +1277,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="C5" t="n">
-        <v>48.87931034482759</v>
+        <v>47.87564766839378</v>
       </c>
     </row>
     <row r="6">
@@ -1498,49 +1290,49 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>29</v>
+        <v>321</v>
       </c>
       <c r="C6" t="n">
-        <v>7.5</v>
+        <v>99.79274611398964</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>184</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>47.58620689655172</v>
+        <v>3.10880829015544</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C8" t="n">
-        <v>46.03448275862069</v>
+        <v>53.16062176165803</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SRISHTI.SRISHTI</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="C9" t="n">
-        <v>8.017241379310345</v>
+        <v>30.15544041450777</v>
       </c>
     </row>
     <row r="10">
@@ -1550,49 +1342,62 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="C10" t="n">
-        <v>6.982758620689655</v>
+        <v>34.81865284974093</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>SURESH.DHAWAN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="C11" t="n">
-        <v>42.67241379310344</v>
+        <v>61.86528497409326</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C12" t="n">
-        <v>6.724137931034483</v>
+        <v>26.73575129533679</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>107</v>
+      </c>
+      <c r="C13" t="n">
+        <v>33.26424870466321</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>YATI0689.YATIN</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>170</v>
-      </c>
-      <c r="C13" t="n">
-        <v>43.96551724137931</v>
+      <c r="B14" t="n">
+        <v>42</v>
+      </c>
+      <c r="C14" t="n">
+        <v>13.05699481865285</v>
       </c>
     </row>
   </sheetData>
@@ -1606,7 +1411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1633,7 +1438,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
@@ -1643,367 +1448,277 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>165</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AHMAD.ALMOHAMMED</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>78</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AHME0710.JUBRAN</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>219</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>175</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>106</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DAT0626.LIEN</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>ESSE0616.UDEH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EDGAR.JIMENEZ</t>
+          <t>INUK4091.QAVAVAU</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>221</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EDIT0625.DELACRUZ</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>82</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EDIT0934.TUPINO</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>61</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ESSE0616.UDEH</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>223</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>FAEZ.MORADZADEH</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>86</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GIGNESH.PATEL</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>74</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HARDEEP.CHAUHAN</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>95</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>104</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>57</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>SEPIDEH.AZARIHASHJIN</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>196</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>96</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>SURESH.DHAWAN</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>107</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>130</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MEHD4790.FOURATI</t>
+          <t>TUSHAR.BHATIA</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>45</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>100</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>YATI0689.YATIN</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>125</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SRISHTI.SRISHTI</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>97</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>TARANPREET.KAUR</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>VICENTE.LIM</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>WESL5337.CADETTE</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>WILDINE.JEUNE</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>ZAHIDGUL.MINHAS</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>ZEINAB.MALEKMOHAMMADI</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2057,13 +1772,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-3</v>
+        <v>-27</v>
       </c>
       <c r="C2" t="n">
-        <v>-87</v>
+        <v>-24</v>
       </c>
       <c r="D2" t="n">
-        <v>-359</v>
+        <v>-468</v>
       </c>
       <c r="E2" t="n">
         <v>-1</v>
@@ -2074,16 +1789,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-46</v>
+        <v>-41</v>
       </c>
       <c r="C3" t="n">
-        <v>-248</v>
+        <v>-130</v>
       </c>
       <c r="D3" t="n">
-        <v>-461</v>
+        <v>-788</v>
       </c>
       <c r="E3" t="n">
-        <v>-62</v>
+        <v>-81</v>
       </c>
     </row>
     <row r="4">
@@ -2091,16 +1806,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-92</v>
+        <v>-32</v>
       </c>
       <c r="C4" t="n">
-        <v>-170</v>
+        <v>-168</v>
       </c>
       <c r="D4" t="n">
-        <v>-399</v>
+        <v>-645</v>
       </c>
       <c r="E4" t="n">
-        <v>-143</v>
+        <v>-357</v>
       </c>
     </row>
     <row r="5">
@@ -2108,16 +1823,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-14</v>
+        <v>-10</v>
       </c>
       <c r="C5" t="n">
-        <v>-93</v>
+        <v>-43</v>
       </c>
       <c r="D5" t="n">
-        <v>-411</v>
+        <v>-104</v>
       </c>
       <c r="E5" t="n">
-        <v>-506</v>
+        <v>-156</v>
       </c>
     </row>
     <row r="6">
@@ -2127,16 +1842,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-155</v>
+        <v>-110</v>
       </c>
       <c r="C6" t="n">
-        <v>-598</v>
+        <v>-365</v>
       </c>
       <c r="D6" t="n">
-        <v>-1630</v>
+        <v>-2005</v>
       </c>
       <c r="E6" t="n">
-        <v>-712</v>
+        <v>-595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added resolve count to affect idle time
</commit_message>
<xml_diff>
--- a/output/processed_data.xlsx
+++ b/output/processed_data.xlsx
@@ -1411,7 +1411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1564,161 +1564,191 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MARI882N.ABDELKADER</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>131</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>26</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>60</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>OMAR6689.KHAN</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>162</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PRINCE.FORSON</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>63</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SEPIDEH.AZARIHASHJIN</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>RARG046N.YEBOAH</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>54</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SURESH.DHAWAN</t>
+          <t>SEPIDEH.AZARIHASHJIN</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>133</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>TUSHAR.BHATIA</t>
+          <t>SURESH.DHAWAN</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>68</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>TUSHAR.BHATIA</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>YATI0689.YATIN</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>140</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ZAHIDGUL.MINHAS</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="B32" t="n">
         <v>83</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1772,16 +1802,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-27</v>
+        <v>27</v>
       </c>
       <c r="C2" t="n">
-        <v>-24</v>
+        <v>24</v>
       </c>
       <c r="D2" t="n">
-        <v>-468</v>
+        <v>468</v>
       </c>
       <c r="E2" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1789,16 +1819,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-41</v>
+        <v>41</v>
       </c>
       <c r="C3" t="n">
-        <v>-130</v>
+        <v>130</v>
       </c>
       <c r="D3" t="n">
-        <v>-788</v>
+        <v>788</v>
       </c>
       <c r="E3" t="n">
-        <v>-81</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
@@ -1806,16 +1836,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-32</v>
+        <v>32</v>
       </c>
       <c r="C4" t="n">
-        <v>-168</v>
+        <v>168</v>
       </c>
       <c r="D4" t="n">
-        <v>-645</v>
+        <v>645</v>
       </c>
       <c r="E4" t="n">
-        <v>-357</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5">
@@ -1823,16 +1853,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>-43</v>
+        <v>43</v>
       </c>
       <c r="D5" t="n">
-        <v>-104</v>
+        <v>104</v>
       </c>
       <c r="E5" t="n">
-        <v>-156</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6">
@@ -1842,16 +1872,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-110</v>
+        <v>110</v>
       </c>
       <c r="C6" t="n">
-        <v>-365</v>
+        <v>365</v>
       </c>
       <c r="D6" t="n">
-        <v>-2005</v>
+        <v>2005</v>
       </c>
       <c r="E6" t="n">
-        <v>-595</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did some changes to regular pick
</commit_message>
<xml_diff>
--- a/output/processed_data.xlsx
+++ b/output/processed_data.xlsx
@@ -489,16 +489,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>87</v>
+        <v>178</v>
       </c>
       <c r="D2" t="n">
-        <v>359</v>
+        <v>523</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3">
@@ -506,16 +506,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>248</v>
+        <v>436</v>
       </c>
       <c r="D3" t="n">
-        <v>461</v>
+        <v>664</v>
       </c>
       <c r="E3" t="n">
-        <v>62</v>
+        <v>805</v>
       </c>
     </row>
     <row r="4">
@@ -523,16 +523,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="C4" t="n">
-        <v>170</v>
+        <v>323</v>
       </c>
       <c r="D4" t="n">
-        <v>399</v>
+        <v>604</v>
       </c>
       <c r="E4" t="n">
-        <v>143</v>
+        <v>748</v>
       </c>
     </row>
     <row r="5">
@@ -540,16 +540,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="D5" t="n">
-        <v>411</v>
+        <v>693</v>
       </c>
       <c r="E5" t="n">
-        <v>506</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6">
@@ -559,16 +559,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>155</v>
+        <v>18</v>
       </c>
       <c r="C6" t="n">
-        <v>598</v>
+        <v>1078</v>
       </c>
       <c r="D6" t="n">
-        <v>1630</v>
+        <v>2484</v>
       </c>
       <c r="E6" t="n">
-        <v>712</v>
+        <v>2400</v>
       </c>
     </row>
   </sheetData>
@@ -612,10 +612,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="C2" t="n">
-        <v>165</v>
+        <v>660</v>
       </c>
     </row>
     <row r="3">
@@ -623,10 +623,10 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="C3" t="n">
-        <v>258</v>
+        <v>825</v>
       </c>
     </row>
     <row r="4">
@@ -634,10 +634,10 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>245</v>
+        <v>316</v>
       </c>
       <c r="C4" t="n">
-        <v>214</v>
+        <v>593</v>
       </c>
     </row>
     <row r="5">
@@ -645,10 +645,10 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C5" t="n">
-        <v>110</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6">
@@ -658,10 +658,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>677</v>
+        <v>722</v>
       </c>
       <c r="C6" t="n">
-        <v>747</v>
+        <v>2259</v>
       </c>
     </row>
   </sheetData>
@@ -675,7 +675,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -702,77 +702,97 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>205</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1Y</t>
+          <t>1G</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>156</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2E</t>
+          <t>2D</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3H</t>
+          <t>3D</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>65</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1A</t>
+          <t>2R</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1G</t>
+          <t>2H</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>84</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>3R</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1D</t>
+          <t>2E</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>62</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>3F</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>3H</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -786,7 +806,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -819,237 +839,413 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>AMANDEEP.KAUR3</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>155</v>
+        <v>216</v>
       </c>
       <c r="C2" t="n">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="D2" t="n">
-        <v>178.85</v>
+        <v>128.32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>LOVEDEEP.SINGH</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C3" t="n">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D3" t="n">
-        <v>173.14</v>
+        <v>118.64</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>YATI0689.YATIN</t>
+          <t>PRAJWAL.SINGH14607</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>95</v>
+        <v>154</v>
       </c>
       <c r="C4" t="n">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="D4" t="n">
-        <v>162.86</v>
+        <v>118.46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>150</v>
+        <v>215</v>
       </c>
       <c r="C5" t="n">
-        <v>59</v>
+        <v>122</v>
       </c>
       <c r="D5" t="n">
-        <v>152.54</v>
+        <v>105.74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>RAMI9087.SAIHI</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>97</v>
+        <v>195</v>
       </c>
       <c r="C6" t="n">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="D6" t="n">
-        <v>118.78</v>
+        <v>105.41</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>OLUMIDE.SANUSI</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>352</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>104.55</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AHME0710.JUBRAN</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>102.96</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DAT0626.LIEN</t>
+          <t>FREDRICK.ADEBOGUN</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>249</v>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>176</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>84.89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EDIT0625.DELACRUZ</t>
+          <t>DJOUMA.KOSSI.MAHAMAT.ALI</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>83.27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EDIT0934.TUPINO</t>
+          <t>ABDRAMANE.YAYA.BECHIR</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8</v>
+        <v>209</v>
       </c>
       <c r="C11" t="n">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>81.95999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>MIRYAMIN.ALI14605</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>76.36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>SUSHMITA.PAUL</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>66.23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>HAMID.ABDOULAYE.MAHAMAT</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C14" t="n">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>61.09</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>CHOROMA.ADOUM.BAYE</t>
         </is>
       </c>
       <c r="B15" t="n">
+        <v>73</v>
+      </c>
+      <c r="C15" t="n">
+        <v>91</v>
+      </c>
+      <c r="D15" t="n">
+        <v>48.13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>AGNE8120.CARUTH</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="n">
+        <v>37</v>
+      </c>
+      <c r="D16" t="n">
+        <v>24.32</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>IRENEMAE.CABRERA</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" t="n">
         <v>6</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>LOANA.MBONGO</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>OMAR2415.BAHAMID</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>9</v>
+      </c>
+      <c r="C19" t="n">
+        <v>6</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>PATI2298.ATSIANGBE</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>27</v>
+      </c>
+      <c r="C20" t="n">
         <v>10</v>
       </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>PATR5027.AMEH</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>FATEMEH.EBRAHIMI</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C22" t="n">
+        <v>5</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>SARVJEET.SINGH14910</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>37</v>
+      </c>
+      <c r="C23" t="n">
+        <v>27</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>SONIA.BHARTI</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>8</v>
+      </c>
+      <c r="C24" t="n">
+        <v>3</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>AZAD.KIKI</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>7</v>
+      </c>
+      <c r="C25" t="n">
+        <v>11</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>33</v>
+      </c>
+      <c r="C26" t="n">
+        <v>17</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
         <is>
           <t>Average UPH</t>
         </is>
       </c>
-      <c r="B16" s="1" t="inlineStr"/>
-      <c r="C16" s="1" t="inlineStr"/>
-      <c r="D16" s="1" t="n">
-        <v>157.2</v>
+      <c r="B27" s="1" t="inlineStr"/>
+      <c r="C27" s="1" t="inlineStr"/>
+      <c r="D27" s="1" t="n">
+        <v>87.40000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1063,7 +1259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1096,190 +1292,190 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MARIA.GALDAMEZ</t>
+          <t>MILA1082.PEREZ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>87</v>
+        <v>157</v>
       </c>
       <c r="C2" t="n">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="D2" t="n">
-        <v>100.38</v>
+        <v>61.97</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ASHL1578.PETIQUAY</t>
+          <t>MURSAL.MADADYAR</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C3" t="n">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D3" t="n">
-        <v>75.92</v>
+        <v>61.85</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GEOR950N.PEREZ</t>
+          <t>ASSANE.NDIAYE</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>113</v>
+        <v>38</v>
       </c>
       <c r="C4" t="n">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="D4" t="n">
-        <v>62.78</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>XYZE1559.MACASIL</t>
+          <t>JASMINECAROLE.NAMEKONG</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>138</v>
+        <v>45</v>
       </c>
       <c r="C5" t="n">
-        <v>171</v>
+        <v>91</v>
       </c>
       <c r="D5" t="n">
-        <v>48.42</v>
+        <v>29.67</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PRITTY.MAZUMDER</t>
+          <t>JOSE202N.OSEMWOTA</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="C6" t="n">
-        <v>59</v>
+        <v>178</v>
       </c>
       <c r="D6" t="n">
-        <v>40.68</v>
+        <v>27.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MILA1082.PEREZ</t>
+          <t>FLOYD.MCLEISH</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>162</v>
+        <v>33</v>
       </c>
       <c r="D7" t="n">
-        <v>31.11</v>
+        <v>25.45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RFBASE</t>
+          <t>BLOCHE.BAKELA</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C8" t="n">
-        <v>88</v>
+        <v>160</v>
       </c>
       <c r="D8" t="n">
-        <v>30</v>
+        <v>24.75</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>OMAR2415.BAHAMID</t>
+          <t>MARIO.OUIMET</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C9" t="n">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="D9" t="n">
-        <v>25.61</v>
+        <v>24.26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MATTHEW.BARRETT</t>
+          <t>TOMA9753.LANDUKULUPE</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C10" t="n">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="D10" t="n">
-        <v>21.54</v>
+        <v>23.19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TOMA9753.LANDUKULUPE</t>
+          <t>NANCY.WOOD</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C11" t="n">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="D11" t="n">
-        <v>17.65</v>
+        <v>20.41</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CHEI145N.BOCOUM</t>
+          <t>XYZE1559.MACASIL</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>151</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>20.26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>JOSE202N.OSEMWOTA</t>
+          <t>MELA6559.ROCHETTE</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -1288,14 +1484,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>JOSEPH.MARDINI</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -1304,29 +1500,109 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>CHEI145N.BOCOUM</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>11</v>
+      </c>
+      <c r="C15" t="n">
+        <v>28</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>NICO0711.JANSON</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PATI2298.ATSIANGBE</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CHARLES.VELASCO</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>VINCENTJAY.TABLADA</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>MARY0067.BOULIANNEBL</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>12</v>
-      </c>
-      <c r="C15" t="n">
-        <v>5</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="B20" t="n">
+        <v>9</v>
+      </c>
+      <c r="C20" t="n">
+        <v>6</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
         <is>
           <t>Average UPH</t>
         </is>
       </c>
-      <c r="B16" s="1" t="inlineStr"/>
-      <c r="C16" s="1" t="inlineStr"/>
-      <c r="D16" s="1" t="n">
-        <v>45.4</v>
+      <c r="B21" s="1" t="inlineStr"/>
+      <c r="C21" s="1" t="inlineStr"/>
+      <c r="D21" s="1" t="n">
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
@@ -1340,7 +1616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1377,29 +1653,29 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C2" t="n">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="D2" t="n">
-        <v>84.15000000000001</v>
+        <v>94.65000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ASHL1578.PETIQUAY</t>
+          <t>MURSAL.MADADYAR</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>72</v>
+        <v>174</v>
       </c>
       <c r="C3" t="n">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="D3" t="n">
-        <v>69.68000000000001</v>
+        <v>89.23</v>
       </c>
     </row>
     <row r="4">
@@ -1409,201 +1685,281 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>139</v>
+        <v>232</v>
       </c>
       <c r="C4" t="n">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="D4" t="n">
-        <v>65.67</v>
+        <v>84.88</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CHEI145N.BOCOUM</t>
+          <t>REX.GOTERA</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>76</v>
+        <v>260</v>
       </c>
       <c r="C5" t="n">
-        <v>77</v>
+        <v>195</v>
       </c>
       <c r="D5" t="n">
-        <v>59.22</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NICO0711.JANSON</t>
+          <t>MELA6559.ROCHETTE</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>31</v>
+        <v>166</v>
       </c>
       <c r="C6" t="n">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="D6" t="n">
-        <v>50.27</v>
+        <v>72.17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>JOSE202N.OSEMWOTA</t>
+          <t>NICO0711.JANSON</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="C7" t="n">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="D7" t="n">
-        <v>36.47</v>
+        <v>68.20999999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ANJALI.BAKSHI</t>
+          <t>TOMA9753.LANDUKULUPE</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>64.62</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DAVI129N.TEJA</t>
+          <t>CHEI145N.BOCOUM</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>62.82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EZRA.RAMIREZ</t>
+          <t>ASSANE.NDIAYE</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>62.45</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>JOSEPH.MARDINI</t>
+          <t>JASMINECAROLE.NAMEKONG</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="C11" t="n">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>59.31</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>KARL.DARANTINAO</t>
+          <t>SHUSHIL.RAI14750</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10</v>
+        <v>185</v>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>189</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>58.73</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>OMAR2415.BAHAMID</t>
+          <t>VINCENTJAY.TABLADA</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>22</v>
+        <v>130</v>
       </c>
       <c r="C13" t="n">
-        <v>19</v>
+        <v>151</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>51.66</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PRITTY.MAZUMDER</t>
+          <t>ABDULLAH.SALEM.AHMED.BARH</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="C14" t="n">
-        <v>11</v>
+        <v>117</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>49.23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TOMA9753.LANDUKULUPE</t>
+          <t>ZULQERNAIN.SHAIKH</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="C15" t="n">
-        <v>29</v>
+        <v>181</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>41.44</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>JOEL.NAPOLEON</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>112</v>
+      </c>
+      <c r="C16" t="n">
+        <v>165</v>
+      </c>
+      <c r="D16" t="n">
+        <v>40.73</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>MONCEF.BOUKHOUDMI</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>68</v>
+      </c>
+      <c r="C17" t="n">
+        <v>103</v>
+      </c>
+      <c r="D17" t="n">
+        <v>39.61</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>FLOYD.MCLEISH</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>23</v>
+      </c>
+      <c r="C18" t="n">
+        <v>38</v>
+      </c>
+      <c r="D18" t="n">
+        <v>36.32</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>NANCY.WOOD</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>7</v>
+      </c>
+      <c r="C19" t="n">
+        <v>16</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>JOSE202N.OSEMWOTA</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
         <is>
           <t>Average UPH</t>
         </is>
       </c>
-      <c r="B16" s="1" t="inlineStr"/>
-      <c r="C16" s="1" t="inlineStr"/>
-      <c r="D16" s="1" t="n">
-        <v>60.9</v>
+      <c r="B21" s="1" t="inlineStr"/>
+      <c r="C21" s="1" t="inlineStr"/>
+      <c r="D21" s="1" t="n">
+        <v>62.1</v>
       </c>
     </row>
   </sheetData>
@@ -1617,7 +1973,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1645,118 +2001,105 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>GAGA4290.KALSI</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>4.913793103448276</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>IRENEMAE.CABRERA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7758620689655172</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EDGAR.JIMENEZ</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5172413793103449</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GIGNESH.PATEL</t>
+          <t>MOHAMMED.MAHMOOD</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2586206896551724</v>
+        <v>0.5333333333333333</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>NAWAF.HAGE.CHEHADE</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>5.431034482758621</v>
+        <v>1.866666666666667</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>PATI2298.ATSIANGBE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1.810344827586207</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>22.75862068965517</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>YASER.KABOUDANI</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>3.103448275862069</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ZAHIDGUL.MINHAS</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.5172413793103449</v>
+        <v>0.5333333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -1770,7 +2113,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1803,190 +2146,190 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>161</v>
       </c>
       <c r="C2" t="n">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="D2" t="n">
-        <v>93.2</v>
+        <v>122.3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>YASER.KABOUDANI</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>45</v>
+        <v>134</v>
       </c>
       <c r="C3" t="n">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="D3" t="n">
-        <v>81.8</v>
+        <v>114.9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>MOHAMMED.SALEM</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="C4" t="n">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D4" t="n">
-        <v>74.59999999999999</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>YATI0689.YATIN</t>
+          <t>WIDLINE.JEUNE</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="C5" t="n">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="D5" t="n">
-        <v>63.7</v>
+        <v>94.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SRISHTI.SRISHTI</t>
+          <t>KANIKA.KANIKA14970</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C6" t="n">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D6" t="n">
-        <v>62.7</v>
+        <v>81.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GIGNESH.PATEL</t>
+          <t>MURLIMANOHAR.MOTWANIBHATI</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C7" t="n">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="D7" t="n">
-        <v>59.5</v>
+        <v>78.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>OMAR.BAHAMID</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="C8" t="n">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="D8" t="n">
-        <v>58.5</v>
+        <v>65.90000000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FAEZ.MORADZADEH</t>
+          <t>NAWAF.HAGE.CHEHADE</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C9" t="n">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D9" t="n">
-        <v>38.6</v>
+        <v>64.90000000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>HARDEEP.CHAUHAN</t>
+          <t>HAMID.ABDOULAYE.MAHAMAT</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C10" t="n">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D10" t="n">
-        <v>33.9</v>
+        <v>55.1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ZEINAB.MALEKMOHAMMADI</t>
+          <t>OUMAR.DIOP</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C11" t="n">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D11" t="n">
-        <v>33.1</v>
+        <v>41.2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>VICENTE.LIM</t>
+          <t>ARSENE.LOULENDO</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="n">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D12" t="n">
-        <v>24.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AHMAD.ALMOHAMMED</t>
+          <t>SIMRAN.SIMRAN14162</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -1995,14 +2338,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>MOHAMMED.MAHMOOD</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C14" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -2011,14 +2354,14 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>BOUBA.BAKARI.ALI</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -2027,14 +2370,14 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>MAMADOU.ADAMS.BARRY</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C16" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -2043,29 +2386,77 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
+          <t>MACLY.BEAUBRUN</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>KOMALDEEP.KAUR14903</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>38</v>
+      </c>
+      <c r="C18" t="n">
+        <v>25</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CARL.NITCHELL.LUCCE</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>38</v>
+      </c>
+      <c r="C19" t="n">
+        <v>25</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>YEVA.NAZARKINA</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>11</v>
+      </c>
+      <c r="C20" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
         <is>
           <t>Average UPH</t>
         </is>
       </c>
-      <c r="B18" s="1" t="inlineStr"/>
-      <c r="C18" s="1" t="inlineStr"/>
-      <c r="D18" s="1" t="n">
-        <v>56.8</v>
+      <c r="B21" s="1" t="inlineStr"/>
+      <c r="C21" s="1" t="inlineStr"/>
+      <c r="D21" s="1" t="n">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2112,382 +2503,382 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TARANPREET.KAUR</t>
+          <t>KANIKA.KANIKA14970</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="C2" t="n">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="D2" t="n">
-        <v>94.8</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>SONIA.BHARTI</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>172</v>
+        <v>106</v>
       </c>
       <c r="C3" t="n">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="D3" t="n">
-        <v>89</v>
+        <v>92.2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MEHD4790.FOURATI</t>
+          <t>YASER.KABOUDANI</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>258</v>
+        <v>85</v>
       </c>
       <c r="C4" t="n">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="D4" t="n">
-        <v>85.5</v>
+        <v>86.40000000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>MOHAMMED.MAHMOOD</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>64</v>
+        <v>191</v>
       </c>
       <c r="C5" t="n">
-        <v>56</v>
+        <v>133</v>
       </c>
       <c r="D5" t="n">
-        <v>68.59999999999999</v>
+        <v>86.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>WIDLINE.JEUNE</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="C6" t="n">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="D6" t="n">
-        <v>66.8</v>
+        <v>85.90000000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>MOHAMMED.SALEM</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C7" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D7" t="n">
-        <v>65.5</v>
+        <v>81.40000000000001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>KOMALDEEP.KAUR14903</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="C8" t="n">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="D8" t="n">
-        <v>63.6</v>
+        <v>79.40000000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>HAMID.ABDOULAYE.MAHAMAT</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C9" t="n">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D9" t="n">
-        <v>56.8</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>YEVA.NAZARKINA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>106</v>
+        <v>196</v>
       </c>
       <c r="C10" t="n">
-        <v>112</v>
+        <v>161</v>
       </c>
       <c r="D10" t="n">
-        <v>56.8</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>MURLIMANOHAR.MOTWANIBHATI</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="C11" t="n">
-        <v>122</v>
+        <v>80</v>
       </c>
       <c r="D11" t="n">
-        <v>56.1</v>
+        <v>72.8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>OMAR.BAHAMID</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C12" t="n">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D12" t="n">
-        <v>54.5</v>
+        <v>69.2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
+          <t>GAGA4290.KALSI</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C13" t="n">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="D13" t="n">
-        <v>53.5</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>NAWAF.HAGE.CHEHADE</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="C14" t="n">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D14" t="n">
-        <v>50.4</v>
+        <v>64.90000000000001</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>MUSKANPREET.KAUR</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="C15" t="n">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D15" t="n">
-        <v>37.3</v>
+        <v>60.6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>MAMADOU.ADAMS.BARRY</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="C16" t="n">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="D16" t="n">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>SIMRAN.SIMRAN14162</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="C17" t="n">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GIGNESH.PATEL</t>
+          <t>ARSENE.LOULENDO</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12</v>
+        <v>149</v>
       </c>
       <c r="C18" t="n">
-        <v>8</v>
+        <v>175</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>51.1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>EDIT0934.TUPINO</t>
+          <t>MIKAEL.SAMUEL</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C19" t="n">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>49.9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>CARL.NITCHELL.LUCCE</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12</v>
+        <v>90</v>
       </c>
       <c r="C20" t="n">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>46.2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>EDIT0625.DELACRUZ</t>
+          <t>SAJEELUR.REHMAN15006</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>45.2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>OUMAR.DIOP</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C22" t="n">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>41.2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>BOUBA.BAKARI.ALI</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="C23" t="n">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>DAT0626.LIEN</t>
+          <t>MACLY.BEAUBRUN</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="C24" t="n">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>37.6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>YATI0689.YATIN</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -2496,14 +2887,14 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C26" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -2518,7 +2909,7 @@
       <c r="B27" s="1" t="inlineStr"/>
       <c r="C27" s="1" t="inlineStr"/>
       <c r="D27" s="1" t="n">
-        <v>62.3</v>
+        <v>66.09999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2532,7 +2923,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2560,157 +2951,300 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>ABDRAMANE.YAYA.BECHIR</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>120</v>
+        <v>59</v>
       </c>
       <c r="C2" t="n">
-        <v>31.03448275862069</v>
+        <v>15.73333333333333</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>16.55172413793104</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>AMANDEEP.KAUR3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="C4" t="n">
-        <v>25.86206896551724</v>
+        <v>40.53333333333333</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>CHOROMA.ADOUM.BAYE</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>189</v>
+        <v>55</v>
       </c>
       <c r="C5" t="n">
-        <v>48.87931034482759</v>
+        <v>14.66666666666667</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ESSE0616.UDEH</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" t="n">
-        <v>7.5</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>DJOUMA.KOSSI.MAHAMAT.ALI</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="C7" t="n">
-        <v>47.58620689655172</v>
+        <v>39.73333333333333</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>GAGA4290.KALSI</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>178</v>
+        <v>13</v>
       </c>
       <c r="C8" t="n">
-        <v>46.03448275862069</v>
+        <v>3.466666666666667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SRISHTI.SRISHTI</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="C9" t="n">
-        <v>8.017241379310345</v>
+        <v>42.13333333333333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>KHINEHAYMAR.THAUNG</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>6.982758620689655</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>LOVEDEEP.SINGH</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>165</v>
+        <v>261</v>
       </c>
       <c r="C11" t="n">
-        <v>42.67241379310344</v>
+        <v>69.59999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C12" t="n">
-        <v>6.724137931034483</v>
+        <v>5.866666666666666</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>MARY0067.BOULIANNEBL</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.2666666666666667</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MIRYAMIN.ALI14605</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>72</v>
+      </c>
+      <c r="C14" t="n">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>OMAR2415.BAHAMID</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.2666666666666667</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>PATI2298.ATSIANGBE</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.2666666666666667</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PRAJWAL.SINGH14607</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>130</v>
+      </c>
+      <c r="C17" t="n">
+        <v>34.66666666666666</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>RAMI9087.SAIHI</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>49</v>
+      </c>
+      <c r="C18" t="n">
+        <v>13.06666666666667</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>SARVJEET.SINGH14910</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>344</v>
+      </c>
+      <c r="C19" t="n">
+        <v>91.73333333333333</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SONIA.BHARTI</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>176</v>
+      </c>
+      <c r="C20" t="n">
+        <v>46.93333333333333</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SUSHMITA.PAUL</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>167</v>
+      </c>
+      <c r="C21" t="n">
+        <v>44.53333333333333</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>WIDLINE.JEUNE</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>30</v>
+      </c>
+      <c r="C22" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>YATI0689.YATIN</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>170</v>
-      </c>
-      <c r="C13" t="n">
-        <v>43.96551724137931</v>
+      <c r="B23" t="n">
+        <v>398</v>
+      </c>
+      <c r="C23" t="n">
+        <v>106.1333333333333</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ZAHIDGUL.MINHAS</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>4</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.066666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -2724,7 +3258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2747,11 +3281,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>ABDRAMANE.YAYA.BECHIR</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
@@ -2761,67 +3295,67 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>159</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AHMAD.ALMOHAMMED</t>
+          <t>AMANDEEP.KAUR3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>78</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AHME0710.JUBRAN</t>
+          <t>ARSENE.LOULENDO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>219</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>AZAD.KIKI</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>175</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>BOUBA.BAKARI.ALI</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>106</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DAT0626.LIEN</t>
+          <t>CARL.NITCHELL.LUCCE</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>CHOROMA.ADOUM.BAYE</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10">
@@ -2831,157 +3365,157 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EDGAR.JIMENEZ</t>
+          <t>DJOUMA.KOSSI.MAHAMAT.ALI</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>221</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EDIT0625.DELACRUZ</t>
+          <t>FATEMEH.EBRAHIMI</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>82</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EDIT0934.TUPINO</t>
+          <t>GAGA4290.KALSI</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>61</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ESSE0616.UDEH</t>
+          <t>HAMID.ABDOULAYE.MAHAMAT</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>223</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>FAEZ.MORADZADEH</t>
+          <t>IRENEMAE.CABRERA</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>86</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GIGNESH.PATEL</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>74</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HARDEEP.CHAUHAN</t>
+          <t>KANIKA.KANIKA14970</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>KHINEHAYMAR.THAUNG</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>104</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>KOMALDEEP.KAUR14903</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>76</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>LOVEDEEP.SINGH</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>182</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>MACLY.BEAUBRUN</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>96</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>MAMADOU.ADAMS.BARRY</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>194</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MEHD4790.FOURATI</t>
+          <t>MARY0067.BOULIANNEBL</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>45</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26">
@@ -2991,147 +3525,257 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>MIKAEL.SAMUEL</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>100</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>MIRYAMIN.ALI14605</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>125</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SRISHTI.SRISHTI</t>
+          <t>MOHAMMED.MAHMOOD</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>97</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>MOHAMMED.SALEM</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>TARANPREET.KAUR</t>
+          <t>MURLIMANOHAR.MOTWANIBHATI</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>117</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>MUSKANPREET.KAUR</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>VICENTE.LIM</t>
+          <t>NAWAF.HAGE.CHEHADE</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>OMAR.BAHAMID</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>64</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>OMAR2415.BAHAMID</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>100</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>YATI0689.YATIN</t>
+          <t>OUMAR.DIOP</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>85</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>PATI2298.ATSIANGBE</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>163</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>99</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ZEINAB.MALEKMOHAMMADI</t>
+          <t>PRAJWAL.SINGH14607</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>63</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>RAMI9087.SAIHI</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>192</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>SAJEELUR.REHMAN15006</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>SARVJEET.SINGH14910</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>SIMRAN.SIMRAN14162</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>SONIA.BHARTI</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>SUSHMITA.PAUL</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>THIE6554.DIALLO</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>WIDLINE.JEUNE</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>YASER.KABOUDANI</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>YEVA.NAZARKINA</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ZAHIDGUL.MINHAS</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes to idle time
</commit_message>
<xml_diff>
--- a/output/processed_data.xlsx
+++ b/output/processed_data.xlsx
@@ -28,7 +28,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -36,8 +36,14 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -48,6 +54,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00ADD8E6"/>
         <bgColor rgb="00ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EEF5FF"/>
+        <bgColor rgb="00EEF5FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -63,9 +75,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -489,16 +513,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>178</v>
+        <v>87</v>
       </c>
       <c r="D2" t="n">
-        <v>523</v>
+        <v>359</v>
       </c>
       <c r="E2" t="n">
-        <v>384</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -506,16 +530,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C3" t="n">
-        <v>436</v>
+        <v>248</v>
       </c>
       <c r="D3" t="n">
-        <v>664</v>
+        <v>461</v>
       </c>
       <c r="E3" t="n">
-        <v>805</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4">
@@ -523,16 +547,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="C4" t="n">
-        <v>323</v>
+        <v>170</v>
       </c>
       <c r="D4" t="n">
-        <v>604</v>
+        <v>399</v>
       </c>
       <c r="E4" t="n">
-        <v>748</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5">
@@ -540,16 +564,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="D5" t="n">
-        <v>693</v>
+        <v>411</v>
       </c>
       <c r="E5" t="n">
-        <v>463</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6">
@@ -559,16 +583,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="C6" t="n">
-        <v>1078</v>
+        <v>598</v>
       </c>
       <c r="D6" t="n">
-        <v>2484</v>
+        <v>1630</v>
       </c>
       <c r="E6" t="n">
-        <v>2400</v>
+        <v>712</v>
       </c>
     </row>
   </sheetData>
@@ -612,10 +636,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="C2" t="n">
-        <v>660</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3">
@@ -623,10 +647,10 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="C3" t="n">
-        <v>825</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4">
@@ -634,10 +658,10 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>316</v>
+        <v>245</v>
       </c>
       <c r="C4" t="n">
-        <v>593</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5">
@@ -645,10 +669,10 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="C5" t="n">
-        <v>181</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
@@ -658,10 +682,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>722</v>
+        <v>677</v>
       </c>
       <c r="C6" t="n">
-        <v>2259</v>
+        <v>747</v>
       </c>
     </row>
   </sheetData>
@@ -675,7 +699,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -702,97 +726,77 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>130</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1G</t>
+          <t>1Y</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>307</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2D</t>
+          <t>2E</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>47</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3D</t>
+          <t>3H</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>221</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2R</t>
+          <t>1A</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>94</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2H</t>
+          <t>1G</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>29</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3R</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2E</t>
+          <t>1D</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>3F</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>3H</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -806,7 +810,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,413 +843,237 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AMANDEEP.KAUR3</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>216</v>
+        <v>155</v>
       </c>
       <c r="C2" t="n">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="D2" t="n">
-        <v>128.32</v>
+        <v>178.85</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>LOVEDEEP.SINGH</t>
+          <t>ADOL798N.SEEMANNVAZQ</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="C3" t="n">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D3" t="n">
-        <v>118.64</v>
+        <v>173.14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PRAJWAL.SINGH14607</t>
+          <t>YATI0689.YATIN</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>154</v>
+        <v>95</v>
       </c>
       <c r="C4" t="n">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="D4" t="n">
-        <v>118.46</v>
+        <v>162.86</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>215</v>
+        <v>150</v>
       </c>
       <c r="C5" t="n">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="D5" t="n">
-        <v>105.74</v>
+        <v>152.54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>195</v>
+        <v>97</v>
       </c>
       <c r="C6" t="n">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="D6" t="n">
-        <v>105.41</v>
+        <v>118.78</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>OLUMIDE.SANUSI</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>352</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>202</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>104.55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>AHME0710.JUBRAN</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>139</v>
+        <v>25</v>
       </c>
       <c r="C8" t="n">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>102.96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FREDRICK.ADEBOGUN</t>
+          <t>DAT0626.LIEN</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>249</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>176</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>84.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DJOUMA.KOSSI.MAHAMAT.ALI</t>
+          <t>EDIT0625.DELACRUZ</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>83.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ABDRAMANE.YAYA.BECHIR</t>
+          <t>EDIT0934.TUPINO</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>153</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>81.95999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MIRYAMIN.ALI14605</t>
+          <t>KHINEHAYMAR.THAUNG</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>76.36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SUSHMITA.PAUL</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>66.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>HAMID.ABDOULAYE.MAHAMAT</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C14" t="n">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="D14" t="n">
-        <v>61.09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CHOROMA.ADOUM.BAYE</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="D15" t="n">
-        <v>48.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>AGNE8120.CARUTH</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>15</v>
-      </c>
-      <c r="C16" t="n">
-        <v>37</v>
-      </c>
-      <c r="D16" t="n">
-        <v>24.32</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>IRENEMAE.CABRERA</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>4</v>
-      </c>
-      <c r="C17" t="n">
-        <v>6</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>LOANA.MBONGO</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>OMAR2415.BAHAMID</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>9</v>
-      </c>
-      <c r="C19" t="n">
-        <v>6</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>PATI2298.ATSIANGBE</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>27</v>
-      </c>
-      <c r="C20" t="n">
-        <v>10</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>PATR5027.AMEH</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>4</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>FATEMEH.EBRAHIMI</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>19</v>
-      </c>
-      <c r="C22" t="n">
-        <v>5</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>SARVJEET.SINGH14910</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>37</v>
-      </c>
-      <c r="C23" t="n">
-        <v>27</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>SONIA.BHARTI</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>8</v>
-      </c>
-      <c r="C24" t="n">
-        <v>3</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>AZAD.KIKI</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>7</v>
-      </c>
-      <c r="C25" t="n">
-        <v>11</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>33</v>
-      </c>
-      <c r="C26" t="n">
-        <v>17</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>Average UPH</t>
         </is>
       </c>
-      <c r="B27" s="1" t="inlineStr"/>
-      <c r="C27" s="1" t="inlineStr"/>
-      <c r="D27" s="1" t="n">
-        <v>87.40000000000001</v>
+      <c r="B16" s="1" t="inlineStr"/>
+      <c r="C16" s="1" t="inlineStr"/>
+      <c r="D16" s="1" t="n">
+        <v>157.2</v>
       </c>
     </row>
   </sheetData>
@@ -1259,7 +1087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1292,190 +1120,190 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MILA1082.PEREZ</t>
+          <t>MARIA.GALDAMEZ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="C2" t="n">
-        <v>152</v>
+        <v>52</v>
       </c>
       <c r="D2" t="n">
-        <v>61.97</v>
+        <v>100.38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MURSAL.MADADYAR</t>
+          <t>ASHL1578.PETIQUAY</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C3" t="n">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D3" t="n">
-        <v>61.85</v>
+        <v>75.92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ASSANE.NDIAYE</t>
+          <t>GEOR950N.PEREZ</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="C4" t="n">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="D4" t="n">
-        <v>38</v>
+        <v>62.78</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>JASMINECAROLE.NAMEKONG</t>
+          <t>XYZE1559.MACASIL</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="C5" t="n">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="D5" t="n">
-        <v>29.67</v>
+        <v>48.42</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>JOSE202N.OSEMWOTA</t>
+          <t>PRITTY.MAZUMDER</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="C6" t="n">
-        <v>178</v>
+        <v>59</v>
       </c>
       <c r="D6" t="n">
-        <v>27.3</v>
+        <v>40.68</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FLOYD.MCLEISH</t>
+          <t>MILA1082.PEREZ</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="C7" t="n">
-        <v>33</v>
+        <v>162</v>
       </c>
       <c r="D7" t="n">
-        <v>25.45</v>
+        <v>31.11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BLOCHE.BAKELA</t>
+          <t>RFBASE</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C8" t="n">
-        <v>160</v>
+        <v>88</v>
       </c>
       <c r="D8" t="n">
-        <v>24.75</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MARIO.OUIMET</t>
+          <t>OMAR2415.BAHAMID</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C9" t="n">
-        <v>141</v>
+        <v>82</v>
       </c>
       <c r="D9" t="n">
-        <v>24.26</v>
+        <v>25.61</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TOMA9753.LANDUKULUPE</t>
+          <t>MATTHEW.BARRETT</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C10" t="n">
-        <v>119</v>
+        <v>39</v>
       </c>
       <c r="D10" t="n">
-        <v>23.19</v>
+        <v>21.54</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NANCY.WOOD</t>
+          <t>TOMA9753.LANDUKULUPE</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C11" t="n">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="D11" t="n">
-        <v>20.41</v>
+        <v>17.65</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>XYZE1559.MACASIL</t>
+          <t>CHEI145N.BOCOUM</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>151</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>20.26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MELA6559.ROCHETTE</t>
+          <t>JOSE202N.OSEMWOTA</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C13" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -1484,14 +1312,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>JOSEPH.MARDINI</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -1500,109 +1328,29 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CHEI145N.BOCOUM</t>
+          <t>MARY0067.BOULIANNEBL</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" t="n">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>NICO0711.JANSON</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>3</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>PATI2298.ATSIANGBE</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>2</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>CHARLES.VELASCO</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>VINCENTJAY.TABLADA</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>MARY0067.BOULIANNEBL</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>9</v>
-      </c>
-      <c r="C20" t="n">
-        <v>6</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>Average UPH</t>
         </is>
       </c>
-      <c r="B21" s="1" t="inlineStr"/>
-      <c r="C21" s="1" t="inlineStr"/>
-      <c r="D21" s="1" t="n">
-        <v>32.5</v>
+      <c r="B16" s="1" t="inlineStr"/>
+      <c r="C16" s="1" t="inlineStr"/>
+      <c r="D16" s="1" t="n">
+        <v>45.4</v>
       </c>
     </row>
   </sheetData>
@@ -1616,7 +1364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1653,29 +1401,29 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C2" t="n">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="D2" t="n">
-        <v>94.65000000000001</v>
+        <v>84.15000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MURSAL.MADADYAR</t>
+          <t>ASHL1578.PETIQUAY</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>174</v>
+        <v>72</v>
       </c>
       <c r="C3" t="n">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="D3" t="n">
-        <v>89.23</v>
+        <v>69.68000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -1685,281 +1433,201 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>232</v>
+        <v>139</v>
       </c>
       <c r="C4" t="n">
-        <v>164</v>
+        <v>127</v>
       </c>
       <c r="D4" t="n">
-        <v>84.88</v>
+        <v>65.67</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>REX.GOTERA</t>
+          <t>CHEI145N.BOCOUM</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>260</v>
+        <v>76</v>
       </c>
       <c r="C5" t="n">
-        <v>195</v>
+        <v>77</v>
       </c>
       <c r="D5" t="n">
-        <v>80</v>
+        <v>59.22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MELA6559.ROCHETTE</t>
+          <t>NICO0711.JANSON</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="C6" t="n">
-        <v>138</v>
+        <v>37</v>
       </c>
       <c r="D6" t="n">
-        <v>72.17</v>
+        <v>50.27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NICO0711.JANSON</t>
+          <t>JOSE202N.OSEMWOTA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="C7" t="n">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="D7" t="n">
-        <v>68.20999999999999</v>
+        <v>36.47</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TOMA9753.LANDUKULUPE</t>
+          <t>ANJALI.BAKSHI</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>64.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CHEI145N.BOCOUM</t>
+          <t>DAVI129N.TEJA</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="C9" t="n">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="D9" t="n">
-        <v>62.82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ASSANE.NDIAYE</t>
+          <t>EZRA.RAMIREZ</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>102</v>
+        <v>7</v>
       </c>
       <c r="C10" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>62.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>JASMINECAROLE.NAMEKONG</t>
+          <t>JOSEPH.MARDINI</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="C11" t="n">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="D11" t="n">
-        <v>59.31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SHUSHIL.RAI14750</t>
+          <t>KARL.DARANTINAO</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>185</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>189</v>
+        <v>9</v>
       </c>
       <c r="D12" t="n">
-        <v>58.73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>VINCENTJAY.TABLADA</t>
+          <t>OMAR2415.BAHAMID</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="C13" t="n">
-        <v>151</v>
+        <v>19</v>
       </c>
       <c r="D13" t="n">
-        <v>51.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ABDULLAH.SALEM.AHMED.BARH</t>
+          <t>PRITTY.MAZUMDER</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C14" t="n">
-        <v>117</v>
+        <v>11</v>
       </c>
       <c r="D14" t="n">
-        <v>49.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ZULQERNAIN.SHAIKH</t>
+          <t>TOMA9753.LANDUKULUPE</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="C15" t="n">
-        <v>181</v>
+        <v>29</v>
       </c>
       <c r="D15" t="n">
-        <v>41.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>JOEL.NAPOLEON</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>112</v>
-      </c>
-      <c r="C16" t="n">
-        <v>165</v>
-      </c>
-      <c r="D16" t="n">
-        <v>40.73</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>MONCEF.BOUKHOUDMI</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>68</v>
-      </c>
-      <c r="C17" t="n">
-        <v>103</v>
-      </c>
-      <c r="D17" t="n">
-        <v>39.61</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>FLOYD.MCLEISH</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>23</v>
-      </c>
-      <c r="C18" t="n">
-        <v>38</v>
-      </c>
-      <c r="D18" t="n">
-        <v>36.32</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>NANCY.WOOD</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>7</v>
-      </c>
-      <c r="C19" t="n">
-        <v>16</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>JOSE202N.OSEMWOTA</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>5</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>Average UPH</t>
         </is>
       </c>
-      <c r="B21" s="1" t="inlineStr"/>
-      <c r="C21" s="1" t="inlineStr"/>
-      <c r="D21" s="1" t="n">
-        <v>62.1</v>
+      <c r="B16" s="1" t="inlineStr"/>
+      <c r="C16" s="1" t="inlineStr"/>
+      <c r="D16" s="1" t="n">
+        <v>60.9</v>
       </c>
     </row>
   </sheetData>
@@ -2001,105 +1669,105 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GAGA4290.KALSI</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8</v>
+        <v>4.913793103448276</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IRENEMAE.CABRERA</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.7758620689655172</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.2586206896551724</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MOHAMMED.MAHMOOD</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5333333333333333</v>
+        <v>5.431034482758621</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NAWAF.HAGE.CHEHADE</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>1.866666666666667</v>
+        <v>1.810344827586207</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2666666666666667</v>
+        <v>22.75862068965517</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2666666666666667</v>
+        <v>3.103448275862069</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>YASER.KABOUDANI</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.5172413793103449</v>
       </c>
     </row>
   </sheetData>
@@ -2113,7 +1781,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2146,190 +1814,190 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>161</v>
+        <v>73</v>
       </c>
       <c r="C2" t="n">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="D2" t="n">
-        <v>122.3</v>
+        <v>93.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>YASER.KABOUDANI</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="C3" t="n">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="D3" t="n">
-        <v>114.9</v>
+        <v>81.8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MOHAMMED.SALEM</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C4" t="n">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D4" t="n">
-        <v>102</v>
+        <v>74.59999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>WIDLINE.JEUNE</t>
+          <t>YATI0689.YATIN</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>146</v>
+        <v>52</v>
       </c>
       <c r="C5" t="n">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="D5" t="n">
-        <v>94.2</v>
+        <v>63.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>KANIKA.KANIKA14970</t>
+          <t>SRISHTI.SRISHTI</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C6" t="n">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D6" t="n">
-        <v>81.3</v>
+        <v>62.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MURLIMANOHAR.MOTWANIBHATI</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C7" t="n">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="D7" t="n">
-        <v>78.2</v>
+        <v>59.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>OMAR.BAHAMID</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C8" t="n">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="D8" t="n">
-        <v>65.90000000000001</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NAWAF.HAGE.CHEHADE</t>
+          <t>FAEZ.MORADZADEH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" t="n">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D9" t="n">
-        <v>64.90000000000001</v>
+        <v>38.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>HAMID.ABDOULAYE.MAHAMAT</t>
+          <t>HARDEEP.CHAUHAN</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C10" t="n">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D10" t="n">
-        <v>55.1</v>
+        <v>33.9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>OUMAR.DIOP</t>
+          <t>ZEINAB.MALEKMOHAMMADI</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C11" t="n">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D11" t="n">
-        <v>41.2</v>
+        <v>33.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ARSENE.LOULENDO</t>
+          <t>VICENTE.LIM</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>24.7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SIMRAN.SIMRAN14162</t>
+          <t>AHMAD.ALMOHAMMED</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -2338,14 +2006,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MOHAMMED.MAHMOOD</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C14" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -2354,14 +2022,14 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BOUBA.BAKARI.ALI</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -2370,14 +2038,14 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MAMADOU.ADAMS.BARRY</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C16" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -2386,77 +2054,29 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MACLY.BEAUBRUN</t>
+          <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>KOMALDEEP.KAUR14903</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>38</v>
-      </c>
-      <c r="C18" t="n">
-        <v>25</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>CARL.NITCHELL.LUCCE</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>38</v>
-      </c>
-      <c r="C19" t="n">
-        <v>25</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>YEVA.NAZARKINA</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>11</v>
-      </c>
-      <c r="C20" t="n">
-        <v>5</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
+      <c r="A18" s="1" t="inlineStr">
         <is>
           <t>Average UPH</t>
         </is>
       </c>
-      <c r="B21" s="1" t="inlineStr"/>
-      <c r="C21" s="1" t="inlineStr"/>
-      <c r="D21" s="1" t="n">
-        <v>82</v>
+      <c r="B18" s="1" t="inlineStr"/>
+      <c r="C18" s="1" t="inlineStr"/>
+      <c r="D18" s="1" t="n">
+        <v>56.8</v>
       </c>
     </row>
   </sheetData>
@@ -2503,382 +2123,382 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>KANIKA.KANIKA14970</t>
+          <t>TARANPREET.KAUR</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="C2" t="n">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>97.8</v>
+        <v>94.8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SONIA.BHARTI</t>
+          <t>IREN797N.CABRERA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>106</v>
+        <v>172</v>
       </c>
       <c r="C3" t="n">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="D3" t="n">
-        <v>92.2</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>YASER.KABOUDANI</t>
+          <t>MEHD4790.FOURATI</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>85</v>
+        <v>258</v>
       </c>
       <c r="C4" t="n">
-        <v>59</v>
+        <v>181</v>
       </c>
       <c r="D4" t="n">
-        <v>86.40000000000001</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MOHAMMED.MAHMOOD</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>191</v>
+        <v>64</v>
       </c>
       <c r="C5" t="n">
-        <v>133</v>
+        <v>56</v>
       </c>
       <c r="D5" t="n">
-        <v>86.2</v>
+        <v>68.59999999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>WIDLINE.JEUNE</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="C6" t="n">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="D6" t="n">
-        <v>85.90000000000001</v>
+        <v>66.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MOHAMMED.SALEM</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C7" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D7" t="n">
-        <v>81.40000000000001</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>KOMALDEEP.KAUR14903</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="C8" t="n">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="D8" t="n">
-        <v>79.40000000000001</v>
+        <v>63.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HAMID.ABDOULAYE.MAHAMAT</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C9" t="n">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D9" t="n">
-        <v>75.5</v>
+        <v>56.8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>YEVA.NAZARKINA</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>196</v>
+        <v>106</v>
       </c>
       <c r="C10" t="n">
-        <v>161</v>
+        <v>112</v>
       </c>
       <c r="D10" t="n">
-        <v>73</v>
+        <v>56.8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MURLIMANOHAR.MOTWANIBHATI</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="C11" t="n">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="D11" t="n">
-        <v>72.8</v>
+        <v>56.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>OMAR.BAHAMID</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C12" t="n">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D12" t="n">
-        <v>69.2</v>
+        <v>54.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GAGA4290.KALSI</t>
+          <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C13" t="n">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="D13" t="n">
-        <v>65</v>
+        <v>53.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>NAWAF.HAGE.CHEHADE</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="C14" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D14" t="n">
-        <v>64.90000000000001</v>
+        <v>50.4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MUSKANPREET.KAUR</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="C15" t="n">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D15" t="n">
-        <v>60.6</v>
+        <v>37.3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MAMADOU.ADAMS.BARRY</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>143</v>
+        <v>42</v>
       </c>
       <c r="C16" t="n">
-        <v>143</v>
+        <v>72</v>
       </c>
       <c r="D16" t="n">
-        <v>60</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SIMRAN.SIMRAN14162</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>132</v>
+        <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="D17" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ARSENE.LOULENDO</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>149</v>
+        <v>12</v>
       </c>
       <c r="C18" t="n">
-        <v>175</v>
+        <v>8</v>
       </c>
       <c r="D18" t="n">
-        <v>51.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MIKAEL.SAMUEL</t>
+          <t>EDIT0934.TUPINO</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C19" t="n">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="D19" t="n">
-        <v>49.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CARL.NITCHELL.LUCCE</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="C20" t="n">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="D20" t="n">
-        <v>46.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SAJEELUR.REHMAN15006</t>
+          <t>EDIT0625.DELACRUZ</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>45.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>OUMAR.DIOP</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C22" t="n">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="D22" t="n">
-        <v>41.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BOUBA.BAKARI.ALI</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="C23" t="n">
-        <v>159</v>
+        <v>14</v>
       </c>
       <c r="D23" t="n">
-        <v>38.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>MACLY.BEAUBRUN</t>
+          <t>DAT0626.LIEN</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>174</v>
+        <v>6</v>
       </c>
       <c r="D24" t="n">
-        <v>37.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>YATI0689.YATIN</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C25" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -2887,14 +2507,14 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>ADOL798N.SEEMANNVAZQ</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -2909,7 +2529,7 @@
       <c r="B27" s="1" t="inlineStr"/>
       <c r="C27" s="1" t="inlineStr"/>
       <c r="D27" s="1" t="n">
-        <v>66.09999999999999</v>
+        <v>62.3</v>
       </c>
     </row>
   </sheetData>
@@ -2923,7 +2543,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2951,300 +2571,157 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ABDRAMANE.YAYA.BECHIR</t>
+          <t>ADOL798N.SEEMANNVAZQ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="C2" t="n">
-        <v>15.73333333333333</v>
+        <v>31.03448275862069</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8</v>
+        <v>16.55172413793104</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AMANDEEP.KAUR3</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>152</v>
+        <v>100</v>
       </c>
       <c r="C4" t="n">
-        <v>40.53333333333333</v>
+        <v>25.86206896551724</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CHOROMA.ADOUM.BAYE</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>55</v>
+        <v>189</v>
       </c>
       <c r="C5" t="n">
-        <v>14.66666666666667</v>
+        <v>48.87931034482759</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>ESSE0616.UDEH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C6" t="n">
-        <v>7.2</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DJOUMA.KOSSI.MAHAMAT.ALI</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="C7" t="n">
-        <v>39.73333333333333</v>
+        <v>47.58620689655172</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GAGA4290.KALSI</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="C8" t="n">
-        <v>3.466666666666667</v>
+        <v>46.03448275862069</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>SRISHTI.SRISHTI</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>158</v>
+        <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>42.13333333333333</v>
+        <v>8.017241379310345</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2666666666666667</v>
+        <v>6.982758620689655</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LOVEDEEP.SINGH</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>261</v>
+        <v>165</v>
       </c>
       <c r="C11" t="n">
-        <v>69.59999999999999</v>
+        <v>42.67241379310344</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C12" t="n">
-        <v>5.866666666666666</v>
+        <v>6.724137931034483</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MARY0067.BOULIANNEBL</t>
+          <t>YATI0689.YATIN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>170</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2666666666666667</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>MIRYAMIN.ALI14605</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>72</v>
-      </c>
-      <c r="C14" t="n">
-        <v>19.2</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>OMAR2415.BAHAMID</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.2666666666666667</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>PATI2298.ATSIANGBE</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.2666666666666667</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>PRAJWAL.SINGH14607</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>130</v>
-      </c>
-      <c r="C17" t="n">
-        <v>34.66666666666666</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>RAMI9087.SAIHI</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>49</v>
-      </c>
-      <c r="C18" t="n">
-        <v>13.06666666666667</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>SARVJEET.SINGH14910</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>344</v>
-      </c>
-      <c r="C19" t="n">
-        <v>91.73333333333333</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>SONIA.BHARTI</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>176</v>
-      </c>
-      <c r="C20" t="n">
-        <v>46.93333333333333</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>SUSHMITA.PAUL</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>167</v>
-      </c>
-      <c r="C21" t="n">
-        <v>44.53333333333333</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>WIDLINE.JEUNE</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>30</v>
-      </c>
-      <c r="C22" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>398</v>
-      </c>
-      <c r="C23" t="n">
-        <v>106.1333333333333</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>ZAHIDGUL.MINHAS</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>4</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1.066666666666667</v>
+        <v>43.96551724137931</v>
       </c>
     </row>
   </sheetData>
@@ -3258,524 +2735,700 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>UserID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>TotalIdleTime</t>
         </is>
       </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>FirstActionTime</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>LastActionTime</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ABDRAMANE.YAYA.BECHIR</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>21</v>
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>ESSE0616.UDEH</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>223</v>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>10:01:00 PM</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>11:46:00 PM</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>AGNE8120.CARUTH</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>139</v>
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>AHME0710.JUBRAN</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>219</v>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>11:39:00 PM</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>11:46:00 PM</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>AMANDEEP.KAUR3</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>BOHD0676.KUSHLIAK</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>175</v>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>08:37:00 PM</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>11:26:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>ADOL798N.SEEMANNVAZQ</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>141</v>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>09:49:00 PM</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>11:42:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>PATR5027.AMEH</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>125</v>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>08:46:00 PM</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>11:20:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>TARANPREET.KAUR</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>117</v>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>09:57:00 PM</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>10:48:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>LOWRHY-OTIENO.JAOKO</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>107</v>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>08:38:00 PM</t>
+        </is>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>11:59:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>BUDD0680.TENNAKOON</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>106</v>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>08:38:00 PM</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>11:47:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>IREN797N.CABRERA</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>104</v>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>08:45:00 PM</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="inlineStr">
+        <is>
+          <t>11:43:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>WILDINE.JEUNE</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>08:38:00 PM</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
+        <is>
+          <t>11:57:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>NESR2403.ATTALAH</t>
+        </is>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>08:46:00 PM</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>11:59:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>ZAKI0190.PHILLIPHORS</t>
+        </is>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>99</v>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>08:40:00 PM</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>11:19:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>SRISHTI.SRISHTI</t>
+        </is>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>97</v>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>08:55:00 PM</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>10:41:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>LOANA.MBONGO</t>
+        </is>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>08:51:00 PM</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="inlineStr">
+        <is>
+          <t>11:59:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>HARDEEP.CHAUHAN</t>
+        </is>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>95</v>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>08:57:00 PM</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="inlineStr">
+        <is>
+          <t>10:45:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>DEVI789.SINGH</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>93</v>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>08:46:00 PM</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="inlineStr">
+        <is>
+          <t>11:59:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>FAEZ.MORADZADEH</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>86</v>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>09:02:00 PM</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>10:33:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>85</v>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>08:45:00 PM</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>11:59:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>EDIT0625.DELACRUZ</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>82</v>
+      </c>
+      <c r="C20" s="5" t="inlineStr">
+        <is>
+          <t>09:01:00 PM</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="inlineStr">
+        <is>
+          <t>09:34:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>AHMAD.ALMOHAMMED</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="n">
+        <v>78</v>
+      </c>
+      <c r="C21" s="5" t="inlineStr">
+        <is>
+          <t>08:53:00 PM</t>
+        </is>
+      </c>
+      <c r="D21" s="5" t="inlineStr">
+        <is>
+          <t>09:46:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>KADE3054.ZONGO</t>
+        </is>
+      </c>
+      <c r="B22" s="4" t="n">
+        <v>76</v>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>08:29:00 PM</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>11:57:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>THIE6554.DIALLO</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>08:28:00 PM</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="inlineStr">
+        <is>
+          <t>11:59:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>GIGNESH.PATEL</t>
+        </is>
+      </c>
+      <c r="B24" s="4" t="n">
+        <v>74</v>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>08:21:00 PM</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="inlineStr">
+        <is>
+          <t>11:55:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>STAN9294.BAUER</t>
+        </is>
+      </c>
+      <c r="B25" s="4" t="n">
+        <v>73</v>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>08:15:00 PM</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>11:58:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr">
+        <is>
+          <t>DIAN4065.ENTRIALGO</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="n">
+        <v>72</v>
+      </c>
+      <c r="C26" s="5" t="inlineStr">
+        <is>
+          <t>08:37:00 PM</t>
+        </is>
+      </c>
+      <c r="D26" s="5" t="inlineStr">
+        <is>
+          <t>11:56:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="n">
+        <v>64</v>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
+          <t>08:48:00 PM</t>
+        </is>
+      </c>
+      <c r="D27" s="5" t="inlineStr">
+        <is>
+          <t>11:51:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr">
+        <is>
+          <t>DAT0626.LIEN</t>
+        </is>
+      </c>
+      <c r="B28" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="C28" s="5" t="inlineStr">
+        <is>
+          <t>08:41:00 PM</t>
+        </is>
+      </c>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>09:33:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>ZEINAB.MALEKMOHAMMADI</t>
+        </is>
+      </c>
+      <c r="B29" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>09:03:00 PM</t>
+        </is>
+      </c>
+      <c r="D29" s="5" t="inlineStr">
+        <is>
+          <t>09:56:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="inlineStr">
+        <is>
+          <t>EDIT0934.TUPINO</t>
+        </is>
+      </c>
+      <c r="B30" s="4" t="n">
+        <v>61</v>
+      </c>
+      <c r="C30" s="5" t="inlineStr">
+        <is>
+          <t>08:40:00 PM</t>
+        </is>
+      </c>
+      <c r="D30" s="5" t="inlineStr">
+        <is>
+          <t>09:32:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>JEEW9554.SITUMUDALIG</t>
+        </is>
+      </c>
+      <c r="B31" s="4" t="n">
+        <v>57</v>
+      </c>
+      <c r="C31" s="5" t="inlineStr">
+        <is>
+          <t>08:38:00 PM</t>
+        </is>
+      </c>
+      <c r="D31" s="5" t="inlineStr">
+        <is>
+          <t>11:17:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="inlineStr">
+        <is>
+          <t>VICENTE.LIM</t>
+        </is>
+      </c>
+      <c r="B32" s="4" t="n">
+        <v>55</v>
+      </c>
+      <c r="C32" s="5" t="inlineStr">
+        <is>
+          <t>08:55:00 PM</t>
+        </is>
+      </c>
+      <c r="D32" s="5" t="inlineStr">
+        <is>
+          <t>09:31:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="inlineStr">
+        <is>
+          <t>MEHD4790.FOURATI</t>
+        </is>
+      </c>
+      <c r="B33" s="4" t="n">
         <v>45</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ARSENE.LOULENDO</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>AZAD.KIKI</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>BOUBA.BAKARI.ALI</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>CARL.NITCHELL.LUCCE</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>CHOROMA.ADOUM.BAYE</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>DIAN4065.ENTRIALGO</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>DJOUMA.KOSSI.MAHAMAT.ALI</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>FATEMEH.EBRAHIMI</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>GAGA4290.KALSI</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>HAMID.ABDOULAYE.MAHAMAT</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>IRENEMAE.CABRERA</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>KADE3054.ZONGO</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>KANIKA.KANIKA14970</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>KHINEHAYMAR.THAUNG</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>KOMALDEEP.KAUR14903</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>LOANA.MBONGO</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>LOVEDEEP.SINGH</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>MACLY.BEAUBRUN</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>MAKEDA.OLLIVIERRE</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>MAMADOU.ADAMS.BARRY</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>MARY0067.BOULIANNEBL</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="C33" s="5" t="inlineStr">
+        <is>
+          <t>08:18:00 PM</t>
+        </is>
+      </c>
+      <c r="D33" s="5" t="inlineStr">
+        <is>
+          <t>11:46:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="inlineStr">
         <is>
           <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>MIKAEL.SAMUEL</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>MIRYAMIN.ALI14605</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>MOHAMMED.MAHMOOD</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>MOHAMMED.SALEM</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>MURLIMANOHAR.MOTWANIBHATI</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>MUSKANPREET.KAUR</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>NAWAF.HAGE.CHEHADE</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>OMAR.BAHAMID</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>OMAR2415.BAHAMID</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>OUMAR.DIOP</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>PATI2298.ATSIANGBE</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>PATR5027.AMEH</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>PRAJWAL.SINGH14607</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>RAMI9087.SAIHI</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>SAJEELUR.REHMAN15006</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>SARVJEET.SINGH14910</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>SIMRAN.SIMRAN14162</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>SONIA.BHARTI</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>SUSHMITA.PAUL</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>WIDLINE.JEUNE</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>YASER.KABOUDANI</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>YEVA.NAZARKINA</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>ZAHIDGUL.MINHAS</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>167</v>
+      <c r="B34" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" s="5" t="inlineStr">
+        <is>
+          <t>08:16:00 PM</t>
+        </is>
+      </c>
+      <c r="D34" s="5" t="inlineStr">
+        <is>
+          <t>11:52:00 PM</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>